<commit_message>
update custom theme, ecomme..
</commit_message>
<xml_diff>
--- a/src/plugins/AdvancedCustomPostProAptp/i18n/trans.xlsx
+++ b/src/plugins/AdvancedCustomPostProAptp/i18n/trans.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="155">
   <si>
     <t>Key</t>
   </si>
@@ -69,226 +69,241 @@
     <t>Product Data</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 138</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 139</t>
   </si>
   <si>
     <t>Product type</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 144</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 145</t>
   </si>
   <si>
     <t>Simple Product</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 146</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 147</t>
   </si>
   <si>
     <t>Grouped product</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 147</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 148</t>
   </si>
   <si>
     <t>External/Affiliate product</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 148</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 149</t>
   </si>
   <si>
     <t>Variable product</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 149</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 150</t>
   </si>
   <si>
     <t>Virtual product</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 150</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 151</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 179</t>
   </si>
   <si>
     <t>Downloadable product</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 151</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 152</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 190</t>
   </si>
   <si>
     <t>Price</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 184</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 210</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 61</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 216</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Overview/Overview.js: 12</t>
+  </si>
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 221</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Properties/Properties.js: 152</t>
+  </si>
+  <si>
+    <t>Variations</t>
+  </si>
+  <si>
+    <t>Downloadable</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 226</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 232</t>
+  </si>
+  <si>
+    <t>Shipments</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 237</t>
+  </si>
+  <si>
+    <t>Connected products</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 243</t>
+  </si>
+  <si>
+    <t>Specifications</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 248</t>
+  </si>
+  <si>
+    <t>Question and Answer</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 253</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 258</t>
+  </si>
+  <si>
+    <t>Purchase note</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Advanced/Advanced.js: 18</t>
+  </si>
+  <si>
+    <t>Enable reviews</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Advanced/Advanced.js: 29</t>
+  </si>
+  <si>
+    <t>(New Option)</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Connectedproducts/Connectedproducts.js: 71</t>
+  </si>
+  <si>
+    <t>Up-Selling</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Connectedproducts/Connectedproducts.js: 106</t>
+  </si>
+  <si>
+    <t>Cross-Selling</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Connectedproducts/Connectedproducts.js: 128</t>
+  </si>
+  <si>
+    <t>Downloadable files</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Downloadable/Downloadable.js: 18</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Downloadable/Downloadable.js: 20</t>
+  </si>
+  <si>
+    <t>Download limit</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Downloadable/Downloadable.js: 33</t>
+  </si>
+  <si>
+    <t>Leave blank for unlimited re-downloads.</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Downloadable/Downloadable.js: 34</t>
+  </si>
+  <si>
+    <t>Download expiry</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Downloadable/Downloadable.js: 45</t>
+  </si>
+  <si>
+    <t>Enter the number of days before a download link expires, or leave blank.</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Downloadable/Downloadable.js: 46</t>
+  </si>
+  <si>
+    <t>Product URL</t>
   </si>
   <si>
     <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 46</t>
   </si>
   <si>
-    <t>Overview</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 190</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Overview/Overview.js: 12</t>
-  </si>
-  <si>
-    <t>Properties</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 195</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Properties/Properties.js: 152</t>
-  </si>
-  <si>
-    <t>Variations</t>
-  </si>
-  <si>
-    <t>Downloadable</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 200</t>
-  </si>
-  <si>
-    <t>Warehouse</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 206</t>
-  </si>
-  <si>
-    <t>Shipments</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 211</t>
-  </si>
-  <si>
-    <t>Connected products</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 217</t>
-  </si>
-  <si>
-    <t>Specifications</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 222</t>
-  </si>
-  <si>
-    <t>Question and Answer</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 227</t>
-  </si>
-  <si>
-    <t>Advanced</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData/CreateData.js: 232</t>
-  </si>
-  <si>
-    <t>Purchase note</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Advanced/Advanced.js: 18</t>
-  </si>
-  <si>
-    <t>Enable reviews</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Advanced/Advanced.js: 29</t>
-  </si>
-  <si>
-    <t>(New Option)</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Connectedproducts/Connectedproducts.js: 71</t>
-  </si>
-  <si>
-    <t>Up-Selling</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Connectedproducts/Connectedproducts.js: 106</t>
-  </si>
-  <si>
-    <t>Cross-Selling</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Connectedproducts/Connectedproducts.js: 128</t>
-  </si>
-  <si>
-    <t>Downloadable files</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Downloadable/Downloadable.js: 18</t>
-  </si>
-  <si>
-    <t>Leave blank for unlimited re-downloads.</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Downloadable/Downloadable.js: 19</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Downloadable/Downloadable.js: 35</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Downloadable/Downloadable.js: 21</t>
-  </si>
-  <si>
-    <t>Download limit</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Downloadable/Downloadable.js: 34</t>
-  </si>
-  <si>
-    <t>Download expiry</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Downloadable/Downloadable.js: 46</t>
-  </si>
-  <si>
-    <t>Enter the number of days before a download link expires, or leave blank.</t>
-  </si>
-  <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Downloadable/Downloadable.js: 47</t>
-  </si>
-  <si>
     <t>Compare at Price</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 63</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 78</t>
   </si>
   <si>
     <t>Cost per item</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 80</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 95</t>
   </si>
   <si>
     <t>Customers won’t see this</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 81</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 96</t>
   </si>
   <si>
     <t>Margin</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 98</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 113</t>
   </si>
   <si>
     <t>Profit</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 108</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 123</t>
   </si>
   <si>
     <t>Charge tax on this product</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 149</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 164</t>
+  </si>
+  <si>
+    <t>Tax class</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\General/General.js: 180</t>
   </si>
   <si>
     <t>Custom product attribute</t>
@@ -369,52 +384,64 @@
     <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 20</t>
   </si>
   <si>
+    <t>Manage stock?</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 34</t>
+  </si>
+  <si>
+    <t>Enable stock management at product level</t>
+  </si>
+  <si>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 35</t>
+  </si>
+  <si>
     <t>Quantity</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 31</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 49</t>
   </si>
   <si>
     <t>Stock quantity. If this is a variable product this value will be used to control stock for all variations, unless you define stock at variation level.</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 32</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 50</t>
   </si>
   <si>
     <t>Pre-order allowed?</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 43</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 61</t>
   </si>
   <si>
     <t>Do not allow</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 45</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 63</t>
   </si>
   <si>
     <t>Allowed, but must notify the customer</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 46</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 64</t>
   </si>
   <si>
     <t>If managing inventory, this will control whether to allow pre-orders for products that are out of stock. If enabled, the number of items in stock can be set to a value below zero.</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 49</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 67</t>
   </si>
   <si>
     <t>Out of stock threshold</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 60</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 78</t>
   </si>
   <si>
     <t>When product stock reaches this amount you will be notified by email. It is possible to define different values for each variation individually. The shop default value can be set in Settings &gt; Products &gt; Inventory.</t>
   </si>
   <si>
-    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 62</t>
+    <t>D:\xampp\htdocs\Vn4React\src\plugins\Vn4Ecommerce\PostType\CreateData\components\Warehouse/Warehouse.js: 80</t>
   </si>
   <si>
     <t>English(en_US)</t>
@@ -837,10 +864,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A69" sqref="A69:B69"/>
+      <selection activeCell="A74" sqref="A74:B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -972,427 +999,465 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
         <v>38</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2"/>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
         <v>41</v>
       </c>
-      <c r="B23" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="2"/>
+      <c r="B24" t="s">
         <v>42</v>
-      </c>
-      <c r="B24" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="2"/>
-      <c r="B38" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" t="s">
         <v>71</v>
-      </c>
-      <c r="B39" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" t="s">
         <v>73</v>
-      </c>
-      <c r="B40" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
         <v>75</v>
-      </c>
-      <c r="B41" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" t="s">
         <v>77</v>
-      </c>
-      <c r="B42" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" t="s">
         <v>79</v>
-      </c>
-      <c r="B43" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" t="s">
         <v>81</v>
-      </c>
-      <c r="B44" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" t="s">
         <v>83</v>
-      </c>
-      <c r="B45" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" t="s">
         <v>85</v>
-      </c>
-      <c r="B46" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" t="s">
         <v>87</v>
-      </c>
-      <c r="B47" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" t="s">
         <v>89</v>
-      </c>
-      <c r="B48" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B49" t="s">
         <v>91</v>
-      </c>
-      <c r="B49" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" t="s">
         <v>93</v>
-      </c>
-      <c r="B50" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" t="s">
         <v>95</v>
-      </c>
-      <c r="B51" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" t="s">
         <v>97</v>
-      </c>
-      <c r="B52" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" t="s">
         <v>99</v>
-      </c>
-      <c r="B53" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" t="s">
         <v>101</v>
-      </c>
-      <c r="B54" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" t="s">
         <v>103</v>
-      </c>
-      <c r="B55" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" t="s">
         <v>105</v>
-      </c>
-      <c r="B56" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B57" t="s">
         <v>107</v>
-      </c>
-      <c r="B57" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" t="s">
         <v>109</v>
-      </c>
-      <c r="B58" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" t="s">
         <v>111</v>
-      </c>
-      <c r="B59" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B60" t="s">
         <v>113</v>
-      </c>
-      <c r="B60" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B61" t="s">
         <v>115</v>
-      </c>
-      <c r="B61" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B62" t="s">
         <v>117</v>
-      </c>
-      <c r="B62" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B63" t="s">
         <v>119</v>
-      </c>
-      <c r="B63" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B64" t="s">
         <v>121</v>
-      </c>
-      <c r="B64" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B65" t="s">
         <v>123</v>
-      </c>
-      <c r="B65" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B66" t="s">
         <v>125</v>
-      </c>
-      <c r="B66" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B67" t="s">
         <v>127</v>
-      </c>
-      <c r="B67" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" t="s">
         <v>129</v>
-      </c>
-      <c r="B68" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B69" t="s">
         <v>131</v>
       </c>
-      <c r="B69" t="s">
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="2" t="s">
         <v>132</v>
+      </c>
+      <c r="B70" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B71" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B73" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1411,13 +1476,11 @@
     <mergeCell ref="A12:A12"/>
     <mergeCell ref="A13:A13"/>
     <mergeCell ref="A14:A14"/>
-    <mergeCell ref="A15:A15"/>
-    <mergeCell ref="A16:A16"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A23"/>
-    <mergeCell ref="A24:A24"/>
+    <mergeCell ref="A23:A24"/>
     <mergeCell ref="A25:A25"/>
     <mergeCell ref="A26:A26"/>
     <mergeCell ref="A27:A27"/>
@@ -1430,7 +1493,8 @@
     <mergeCell ref="A34:A34"/>
     <mergeCell ref="A35:A35"/>
     <mergeCell ref="A36:A36"/>
-    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A37:A37"/>
+    <mergeCell ref="A38:A38"/>
     <mergeCell ref="A39:A39"/>
     <mergeCell ref="A40:A40"/>
     <mergeCell ref="A41:A41"/>
@@ -1462,6 +1526,11 @@
     <mergeCell ref="A67:A67"/>
     <mergeCell ref="A68:A68"/>
     <mergeCell ref="A69:A69"/>
+    <mergeCell ref="A70:A70"/>
+    <mergeCell ref="A71:A71"/>
+    <mergeCell ref="A72:A72"/>
+    <mergeCell ref="A73:A73"/>
+    <mergeCell ref="A74:A74"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1482,13 +1551,13 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N65"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1:N65"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1:N69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1514,43 +1583,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -1807,7 +1876,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1825,7 +1894,7 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1843,7 +1912,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1861,7 +1930,7 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1879,7 +1948,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1897,7 +1966,7 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1915,7 +1984,7 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1933,7 +2002,7 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1951,7 +2020,7 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1969,7 +2038,7 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1987,7 +2056,7 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2005,7 +2074,7 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2023,7 +2092,7 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2041,7 +2110,7 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2059,7 +2128,7 @@
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2077,7 +2146,7 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2095,7 +2164,7 @@
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2113,7 +2182,7 @@
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2131,7 +2200,7 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2149,7 +2218,7 @@
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2167,7 +2236,7 @@
     </row>
     <row r="36" spans="1:14">
       <c r="A36" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2185,7 +2254,7 @@
     </row>
     <row r="37" spans="1:14">
       <c r="A37" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -2203,7 +2272,7 @@
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -2221,7 +2290,7 @@
     </row>
     <row r="39" spans="1:14">
       <c r="A39" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2239,7 +2308,7 @@
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2257,7 +2326,7 @@
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -2275,7 +2344,7 @@
     </row>
     <row r="42" spans="1:14">
       <c r="A42" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -2293,7 +2362,7 @@
     </row>
     <row r="43" spans="1:14">
       <c r="A43" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -2311,7 +2380,7 @@
     </row>
     <row r="44" spans="1:14">
       <c r="A44" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -2329,7 +2398,7 @@
     </row>
     <row r="45" spans="1:14">
       <c r="A45" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -2347,7 +2416,7 @@
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -2365,7 +2434,7 @@
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -2383,7 +2452,7 @@
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -2401,7 +2470,7 @@
     </row>
     <row r="49" spans="1:14">
       <c r="A49" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -2419,7 +2488,7 @@
     </row>
     <row r="50" spans="1:14">
       <c r="A50" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -2437,7 +2506,7 @@
     </row>
     <row r="51" spans="1:14">
       <c r="A51" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -2455,7 +2524,7 @@
     </row>
     <row r="52" spans="1:14">
       <c r="A52" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -2473,7 +2542,7 @@
     </row>
     <row r="53" spans="1:14">
       <c r="A53" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -2491,7 +2560,7 @@
     </row>
     <row r="54" spans="1:14">
       <c r="A54" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -2509,7 +2578,7 @@
     </row>
     <row r="55" spans="1:14">
       <c r="A55" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -2527,7 +2596,7 @@
     </row>
     <row r="56" spans="1:14">
       <c r="A56" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -2545,7 +2614,7 @@
     </row>
     <row r="57" spans="1:14">
       <c r="A57" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -2563,7 +2632,7 @@
     </row>
     <row r="58" spans="1:14">
       <c r="A58" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -2581,7 +2650,7 @@
     </row>
     <row r="59" spans="1:14">
       <c r="A59" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -2599,7 +2668,7 @@
     </row>
     <row r="60" spans="1:14">
       <c r="A60" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -2617,7 +2686,7 @@
     </row>
     <row r="61" spans="1:14">
       <c r="A61" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -2635,7 +2704,7 @@
     </row>
     <row r="62" spans="1:14">
       <c r="A62" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -2653,7 +2722,7 @@
     </row>
     <row r="63" spans="1:14">
       <c r="A63" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -2671,7 +2740,7 @@
     </row>
     <row r="64" spans="1:14">
       <c r="A64" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -2689,7 +2758,7 @@
     </row>
     <row r="65" spans="1:14">
       <c r="A65" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -2704,6 +2773,78 @@
       <c r="L65" s="5"/>
       <c r="M65" s="5"/>
       <c r="N65" s="5"/>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5"/>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="A69" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>